<commit_message>
preparation for second pilot. 80 pairs, instruction texts, short break within each city
</commit_message>
<xml_diff>
--- a/stimuli/word_selection.xlsx
+++ b/stimuli/word_selection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zsuzsa\HCCCL\TwoCities\stimuli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zsuzsa\HCCCL\Hippopolis\stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9F63C6-A6B7-46CD-9EBF-5AB3F3655473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9433C50B-A7B5-4E81-A691-4B3C88904584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="163">
   <si>
     <t>HARCSA</t>
   </si>
@@ -434,6 +434,96 @@
   </si>
   <si>
     <t>GYŰRŰ</t>
+  </si>
+  <si>
+    <t>TERASZ</t>
+  </si>
+  <si>
+    <t>PALACK</t>
+  </si>
+  <si>
+    <t>FÜZET</t>
+  </si>
+  <si>
+    <t>TÁSKA</t>
+  </si>
+  <si>
+    <t>MOTOR</t>
+  </si>
+  <si>
+    <t>TÁBLA</t>
+  </si>
+  <si>
+    <t>KERET</t>
+  </si>
+  <si>
+    <t>SZERSZÁM</t>
+  </si>
+  <si>
+    <t>LEVÉL</t>
+  </si>
+  <si>
+    <t>FÜGE</t>
+  </si>
+  <si>
+    <t>KÁRTYA</t>
+  </si>
+  <si>
+    <t>POHÁR</t>
+  </si>
+  <si>
+    <t>ÜVEG</t>
+  </si>
+  <si>
+    <t>ASZTAL</t>
+  </si>
+  <si>
+    <t>FÓKA</t>
+  </si>
+  <si>
+    <t>POLIP</t>
+  </si>
+  <si>
+    <t>TEHÉN</t>
+  </si>
+  <si>
+    <t>PADLÓ</t>
+  </si>
+  <si>
+    <t>TETŐ</t>
+  </si>
+  <si>
+    <t>LIGET</t>
+  </si>
+  <si>
+    <t>TÉRKÉP</t>
+  </si>
+  <si>
+    <t>KORONG</t>
+  </si>
+  <si>
+    <t>FŰRÉSZ</t>
+  </si>
+  <si>
+    <t>PÉKSÉG</t>
+  </si>
+  <si>
+    <t>KIFLI</t>
+  </si>
+  <si>
+    <t>ZSEMLE</t>
+  </si>
+  <si>
+    <t>POGÁCSA</t>
+  </si>
+  <si>
+    <t>TELEP</t>
+  </si>
+  <si>
+    <t>HAJÓ</t>
+  </si>
+  <si>
+    <t>KERÉK</t>
   </si>
 </sst>
 </file>
@@ -994,7 +1084,7 @@
     <cellStyle name="Semleges 2" xfId="9" xr:uid="{4AB7CF26-8EC2-490F-9912-CA46EBCA1A8D}"/>
     <cellStyle name="Számítás 2" xfId="12" xr:uid="{7008B8DE-C5AE-4FC8-B848-A4A3F0E3FCB7}"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1002,96 +1092,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1401,10 +1401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D130"/>
+  <dimension ref="A1:D307"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,7 +1446,7 @@
         <v>69</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B66" si="0">COUNTIF(A3:A301,A3)</f>
+        <f>COUNTIF(A3:A301,A3)</f>
         <v>1</v>
       </c>
       <c r="C3">
@@ -1458,7 +1458,7 @@
         <v>70</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B4:B67" si="0">COUNTIF(A4:A302,A4)</f>
         <v>1</v>
       </c>
       <c r="C4">
@@ -2214,7 +2214,7 @@
         <v>63</v>
       </c>
       <c r="B67">
-        <f t="shared" ref="B67:B130" si="1">COUNTIF(A67:A365,A67)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C67">
@@ -2226,7 +2226,7 @@
         <v>64</v>
       </c>
       <c r="B68">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B68:B131" si="1">COUNTIF(A68:A366,A68)</f>
         <v>1</v>
       </c>
       <c r="C68">
@@ -2839,7 +2839,7 @@
       </c>
       <c r="B119">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C119">
         <v>3</v>
@@ -2977,22 +2977,1192 @@
         <v>2</v>
       </c>
     </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>133</v>
+      </c>
+      <c r="B131">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>134</v>
+      </c>
+      <c r="B132">
+        <f t="shared" ref="B132:B195" si="2">COUNTIF(A132:A430,A132)</f>
+        <v>1</v>
+      </c>
+      <c r="C132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>135</v>
+      </c>
+      <c r="B133">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>136</v>
+      </c>
+      <c r="B134">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>137</v>
+      </c>
+      <c r="B135">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>138</v>
+      </c>
+      <c r="B136">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>139</v>
+      </c>
+      <c r="B137">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>140</v>
+      </c>
+      <c r="B138">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>141</v>
+      </c>
+      <c r="B139">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>142</v>
+      </c>
+      <c r="B140">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>143</v>
+      </c>
+      <c r="B141">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>144</v>
+      </c>
+      <c r="B142">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>145</v>
+      </c>
+      <c r="B143">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>146</v>
+      </c>
+      <c r="B144">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>147</v>
+      </c>
+      <c r="B145">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>148</v>
+      </c>
+      <c r="B146">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>149</v>
+      </c>
+      <c r="B147">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>150</v>
+      </c>
+      <c r="B148">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>151</v>
+      </c>
+      <c r="B149">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>152</v>
+      </c>
+      <c r="B150">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>153</v>
+      </c>
+      <c r="B151">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>154</v>
+      </c>
+      <c r="B152">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>155</v>
+      </c>
+      <c r="B153">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>156</v>
+      </c>
+      <c r="B154">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>157</v>
+      </c>
+      <c r="B155">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>158</v>
+      </c>
+      <c r="B156">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>159</v>
+      </c>
+      <c r="B157">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>160</v>
+      </c>
+      <c r="B158">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>161</v>
+      </c>
+      <c r="B159">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>162</v>
+      </c>
+      <c r="B160">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>120</v>
+      </c>
+      <c r="B161">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B164">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B166">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B168">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B170">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B171">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B172">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B173">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B174">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B175">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B177">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B178">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B179">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B180">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B181">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B182">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B183">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B184">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B185">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B186">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B187">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B188">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B189">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B190">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B191">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B193">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B194">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B195">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B196">
+        <f t="shared" ref="B196:B259" si="3">COUNTIF(A196:A494,A196)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B197">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B198">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B199">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B200">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B201">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B202">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B203">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B204">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B205">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B206">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B207">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B208">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B209">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B210">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B211">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B212">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B213">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B214">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B215">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B216">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B217">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B218">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B219">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B220">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B221">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B222">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B223">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B224">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B225">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B226">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B227">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B228">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B229">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B230">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B231">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B232">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B233">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B234">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B235">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B236">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B237">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B238">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B239">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B240">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B241">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B242">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B243">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B244">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B245">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B246">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B247">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B248">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B249">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B250">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B251">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B252">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B253">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B254">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B255">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B256">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B257">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B258">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B259">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B260">
+        <f t="shared" ref="B260:B307" si="4">COUNTIF(A260:A558,A260)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B261">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B262">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B263">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B264">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B265">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B266">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B267">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B268">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B269">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B270">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B271">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B272">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B273">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B274">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B275">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B276">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B277">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B278">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B279">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B280">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B281">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B282">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B283">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B284">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B285">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B286">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B287">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B288">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B289">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B290">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B291">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B292">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B293">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B294">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B295">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B296">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B297">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B298">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B299">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B300">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B301">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B302">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B303">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B304">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B305">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B306">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B307">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D90">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
deleted test files. corrected position of the break (?)
</commit_message>
<xml_diff>
--- a/stimuli/word_selection.xlsx
+++ b/stimuli/word_selection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zsuzsa\HCCCL\Hippopolis\stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9433C50B-A7B5-4E81-A691-4B3C88904584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECD0578-B8FE-456D-97F8-17E076336FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>HARCSA</t>
   </si>
@@ -524,6 +524,9 @@
   </si>
   <si>
     <t>KERÉK</t>
+  </si>
+  <si>
+    <t>VIHAR</t>
   </si>
 </sst>
 </file>
@@ -1403,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D307"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="A161" sqref="A161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2839,7 +2842,7 @@
       </c>
       <c r="B119">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C119">
         <v>3</v>
@@ -3264,7 +3267,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="B161">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
preparing for student pilot 1. words updated, object images updated, updtae image presentation reduced to 2s, distractor images selected by novelty type.
</commit_message>
<xml_diff>
--- a/stimuli/word_selection.xlsx
+++ b/stimuli/word_selection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zsuzsa\HCCCL\Hippopolis\stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECD0578-B8FE-456D-97F8-17E076336FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C22744-5880-4804-83A4-6C656F1B1D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
   <si>
     <t>HARCSA</t>
   </si>
@@ -527,6 +527,12 @@
   </si>
   <si>
     <t>VIHAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAJTÓ </t>
+  </si>
+  <si>
+    <t>OLDAL</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1086,7 @@
     <cellStyle name="Jó 2" xfId="7" xr:uid="{085FE33D-2CE7-4909-BBFD-86ABFF4CFA07}"/>
     <cellStyle name="Kimenet 2" xfId="11" xr:uid="{3C9428D4-DD2D-47DF-8691-2DC021EB5846}"/>
     <cellStyle name="Magyarázó szöveg 2" xfId="17" xr:uid="{3F1F2AD0-97CB-47EC-B5F2-D5F2359AB6FE}"/>
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normál 2" xfId="1" xr:uid="{E78CBE51-AA73-40C2-8BD9-D1F5C1BE41CD}"/>
     <cellStyle name="Összesen 2" xfId="18" xr:uid="{5DAC51EE-7643-43E2-8589-D605B41E8937}"/>
     <cellStyle name="Rossz 2" xfId="8" xr:uid="{A42D9264-A5C5-48A1-88AF-C4B03A99959D}"/>
@@ -1406,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="A161" sqref="A161"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3275,15 +3281,21 @@
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>164</v>
+      </c>
       <c r="B162">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>165</v>
+      </c>
       <c r="B163">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>